<commit_message>
Add second half of initial IFA design
Vias, drills, and padding still need to be configured.
</commit_message>
<xml_diff>
--- a/specs/ifa-calculations.xlsx
+++ b/specs/ifa-calculations.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey Zheng\Dropbox\HA-HA\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,130 +24,133 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+  <si>
+    <t>Manufacturer</t>
+  </si>
   <si>
     <t>Bay Area Circuits</t>
   </si>
   <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
     <t>Dielectric Material</t>
   </si>
   <si>
+    <t>FR-4</t>
+  </si>
+  <si>
     <t>Dielectric Constant</t>
   </si>
   <si>
-    <t>FR-4</t>
-  </si>
-  <si>
     <t>+/-0.02</t>
   </si>
   <si>
-    <t>Dielectric Constant (eff)</t>
+    <t>Dielectric Height (mils)</t>
+  </si>
+  <si>
+    <t>Frequency (GHz)</t>
+  </si>
+  <si>
+    <t>Effective Wavelength (mm)</t>
+  </si>
+  <si>
+    <t>Effective Wavelength (mils)</t>
+  </si>
+  <si>
+    <t>Trace Height (mils)</t>
+  </si>
+  <si>
+    <t>+/-0.2</t>
   </si>
   <si>
     <t>Reference</t>
   </si>
   <si>
-    <t>Dielectric Height (mils)</t>
-  </si>
-  <si>
-    <t>Frequency (GHz)</t>
-  </si>
-  <si>
-    <t>Effective Wavelength (mm)</t>
-  </si>
-  <si>
-    <t>Effective Wavelength (mils)</t>
-  </si>
-  <si>
-    <t>Trace Height (mils)</t>
-  </si>
-  <si>
-    <t>+/-0.2</t>
+    <t>TI-swru120b.pdf (DN007)</t>
+  </si>
+  <si>
+    <t>Note: Dielectric information and ground/sides dimensions not given.</t>
+  </si>
+  <si>
+    <t>(mm)</t>
+  </si>
+  <si>
+    <t>(mils)</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>W2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>H9</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>W1</t>
   </si>
   <si>
     <t>Actual Design</t>
   </si>
   <si>
-    <t>TI-swru120b.pdf (DN007)</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>H4</t>
-  </si>
-  <si>
-    <t>H5</t>
-  </si>
-  <si>
-    <t>H6</t>
-  </si>
-  <si>
-    <t>H7</t>
-  </si>
-  <si>
-    <t>H8</t>
-  </si>
-  <si>
-    <t>H9</t>
-  </si>
-  <si>
-    <t>W1</t>
-  </si>
-  <si>
-    <t>W2</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>L7</t>
-  </si>
-  <si>
-    <t>L8</t>
-  </si>
-  <si>
-    <t>(mm)</t>
-  </si>
-  <si>
-    <t>(mils)</t>
-  </si>
-  <si>
     <t>Sides</t>
   </si>
   <si>
-    <t>Note: Dielectric information and ground/sides dimensions not given.</t>
+    <t>of effective wavelength</t>
+  </si>
+  <si>
+    <t>Dielectric Constant (Effective)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +162,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,16 +192,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -210,23 +224,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>391708</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>553633</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>10032</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{283B69C1-C117-4680-B761-246AF61803E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF373599-1F67-4A85-9778-5D1AD78785AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -248,7 +262,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7715250" y="2286000"/>
+          <a:off x="7848600" y="2286000"/>
           <a:ext cx="8478433" cy="3629532"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -278,7 +292,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -290,7 +304,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -337,6 +351,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -372,6 +403,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -524,49 +572,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>4.58</v>
@@ -574,89 +619,150 @@
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2">
+        <f>(B3+1)/2+(B3-1)/2*((SQRT(1+12*B6/G14))^-1)</f>
+        <v>4.171349466283643</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
-        <f>(B3+1)/2+(B3-1)/2*((SQRT(1+12*B5/G14))^-1)</f>
-        <v>4.171349466283643</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="2">
+        <v>57</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="2">
+        <f>300000000/(B7*10^6)/SQRT(B4)</f>
+        <v>59.95382315663479</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
-        <v>2.4500000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <f>300000000/(B6*10^6)/SQRT(B4)</f>
-        <v>59.95382315663479</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2">
-        <f>B7*0.0393701*1000</f>
+      <c r="B9" s="2">
+        <f>B8*0.0393701*1000</f>
         <v>2360.3880130590273</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="2">
+        <f>B9/2</f>
+        <v>1180.1940065295137</v>
+      </c>
+      <c r="D9" s="2">
+        <f>B9/4</f>
+        <v>590.09700326475684</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
-        <v>1.9</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2">
         <v>5.7</v>
@@ -666,7 +772,7 @@
         <v>224.40957</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F13" s="2">
         <v>0.46</v>
@@ -675,10 +781,16 @@
         <f>F13*0.0393701*1000</f>
         <v>18.110246</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2">
         <v>0.74</v>
@@ -688,7 +800,7 @@
         <v>29.133873999999999</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F14" s="2">
         <v>25.58</v>
@@ -697,10 +809,22 @@
         <f t="shared" ref="G14:G21" si="1">F14*0.0393701*1000</f>
         <v>1007.0871579999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="1">
+        <f>G14/B9</f>
+        <v>0.42666169817344141</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2">
         <v>1.29</v>
@@ -710,7 +834,7 @@
         <v>50.787429000000003</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2">
         <v>16.399999999999999</v>
@@ -719,10 +843,16 @@
         <f t="shared" si="1"/>
         <v>645.66963999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2">
         <v>2.21</v>
@@ -732,7 +862,7 @@
         <v>87.007920999999982</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F16" s="2">
         <v>2.1800000000000002</v>
@@ -741,10 +871,16 @@
         <f t="shared" si="1"/>
         <v>85.826818000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2">
         <v>0.66</v>
@@ -754,7 +890,7 @@
         <v>25.984265999999998</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F17" s="2">
         <v>4.8</v>
@@ -763,10 +899,16 @@
         <f t="shared" si="1"/>
         <v>188.97647999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2">
         <v>1.21</v>
@@ -776,7 +918,7 @@
         <v>47.637820999999995</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
@@ -785,10 +927,16 @@
         <f t="shared" si="1"/>
         <v>39.370100000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C19" s="2">
         <v>0.8</v>
@@ -798,7 +946,7 @@
         <v>31.496080000000003</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
@@ -807,10 +955,16 @@
         <f t="shared" si="1"/>
         <v>39.370100000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2">
         <v>1.8</v>
@@ -820,7 +974,7 @@
         <v>70.86618</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20" s="2">
         <v>3.2</v>
@@ -829,10 +983,16 @@
         <f t="shared" si="1"/>
         <v>125.98432000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2">
         <v>0.61</v>
@@ -851,10 +1011,16 @@
         <f t="shared" si="1"/>
         <v>17.716545</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2">
         <v>1.21</v>
@@ -863,10 +1029,32 @@
         <f t="shared" si="0"/>
         <v>47.637820999999995</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -874,26 +1062,38 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C26" s="2">
         <f>D26/0.0393701/1000</f>
@@ -903,7 +1103,7 @@
         <v>224</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F26" s="2">
         <f>G26/0.0393701/1000</f>
@@ -912,10 +1112,16 @@
       <c r="G26" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" ref="C27:C35" si="2">D27/0.0393701/1000</f>
@@ -925,7 +1131,7 @@
         <v>29</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" ref="F27:F35" si="3">G27/0.0393701/1000</f>
@@ -934,10 +1140,22 @@
       <c r="G27" s="2">
         <v>1007</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1">
+        <f>G27/B9</f>
+        <v>0.42662477288848083</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="2"/>
@@ -947,7 +1165,7 @@
         <v>51</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="3"/>
@@ -956,10 +1174,16 @@
       <c r="G28" s="2">
         <v>646</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" si="2"/>
@@ -969,7 +1193,7 @@
         <v>87</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="3"/>
@@ -978,10 +1202,16 @@
       <c r="G29" s="2">
         <v>86</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" si="2"/>
@@ -991,7 +1221,7 @@
         <v>26</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="3"/>
@@ -1000,10 +1230,16 @@
       <c r="G30" s="2">
         <v>189</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="2"/>
@@ -1013,7 +1249,7 @@
         <v>28</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="3"/>
@@ -1022,10 +1258,16 @@
       <c r="G31" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="2"/>
@@ -1035,7 +1277,7 @@
         <v>32</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" si="3"/>
@@ -1044,10 +1286,16 @@
       <c r="G32" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C33" s="2">
         <f t="shared" si="2"/>
@@ -1057,7 +1305,7 @@
         <v>71</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" si="3"/>
@@ -1066,10 +1314,16 @@
       <c r="G33" s="2">
         <v>126</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="2"/>
@@ -1088,10 +1342,16 @@
       <c r="G34" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" si="2"/>
@@ -1112,8 +1372,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix via and CPWG calculations
</commit_message>
<xml_diff>
--- a/specs/ifa-calculations.xlsx
+++ b/specs/ifa-calculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>Dielectric Constant (Effective)</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>One row of vias placed 20mils from the keepout, 86.5mils apart from each other, and 19.5mils away from the CPWG.</t>
+  </si>
+  <si>
+    <t>CPWG feedline impedance of 51.84ohm generated with 42mil trace width and 6mil ground spacing on each side.</t>
   </si>
 </sst>
 </file>
@@ -572,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,6 +1380,19 @@
         <v>40</v>
       </c>
     </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1"/>

</xml_diff>